<commit_message>
Testes para a etapa 3 do projeto
</commit_message>
<xml_diff>
--- a/Airpods.xlsx
+++ b/Airpods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liviabn\Documents\Cdados- Projetos\PROJETO1_Cdados\P1Cdados2021_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A732839-CAE8-40DC-8A00-269B3E6FEC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC84B947-8CB3-48DF-8448-283D8519B5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <t>Treinamento</t>
   </si>
   <si>
-    <t xml:space="preserve">Relevância </t>
+    <t>Classificação</t>
   </si>
   <si>
     <t>pqp achei que eu tinha perdido a capinha do airpods e até voltei no supermercado pra procurar essa merda</t>
@@ -2177,7 +2177,7 @@
   <dimension ref="A1:B301"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2187,7 +2187,7 @@
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Revisão da classificação feita
</commit_message>
<xml_diff>
--- a/Airpods.xlsx
+++ b/Airpods.xlsx
@@ -8,20 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liviabn\Documents\Cdados- Projetos\PROJETO1_Cdados\P1Cdados2021_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4872818F-869F-4DBA-80E2-F44F3CF90CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CBF437-3322-4059-B32A-AB84F6575D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
     <sheet name="Teste" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Teste!$B$1:$B$302</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="904">
   <si>
     <t>Treinamento</t>
   </si>
@@ -3147,9 +3150,6 @@
     <t>sorte que comprei airpods pro de r$19,90 no shopee, não curti! haha” 
 economizei 3.000,00 reais. 
 obrigado shopee!</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Classificacao_Teste</t>
@@ -3564,7 +3564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B601"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -3579,7 +3579,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -6591,7 +6591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B302"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -6606,7 +6606,7 @@
         <v>601</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -6633,7 +6633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>605</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>616</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="116" x14ac:dyDescent="0.35">
@@ -6737,7 +6737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>618</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>619</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -6806,7 +6806,7 @@
         <v>626</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -6913,12 +6913,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>640</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -6934,7 +6934,7 @@
         <v>642</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -6942,7 +6942,7 @@
         <v>643</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -6958,7 +6958,7 @@
         <v>645</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -6990,7 +6990,7 @@
         <v>649</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -7161,7 +7161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>671</v>
       </c>
@@ -7169,7 +7169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>672</v>
       </c>
@@ -7241,7 +7241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>681</v>
       </c>
@@ -7254,7 +7254,7 @@
         <v>682</v>
       </c>
       <c r="B82">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -7414,7 +7414,7 @@
         <v>702</v>
       </c>
       <c r="B102">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="116" x14ac:dyDescent="0.35">
@@ -7526,7 +7526,7 @@
         <v>716</v>
       </c>
       <c r="B116">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -7561,7 +7561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>721</v>
       </c>
@@ -7577,7 +7577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>723</v>
       </c>
@@ -7734,10 +7734,10 @@
         <v>742</v>
       </c>
       <c r="B142">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
         <v>743</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>745</v>
       </c>
       <c r="B145">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="58" x14ac:dyDescent="0.35">
@@ -7766,7 +7766,7 @@
         <v>746</v>
       </c>
       <c r="B146">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
@@ -7822,7 +7822,7 @@
         <v>753</v>
       </c>
       <c r="B153">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
@@ -7857,7 +7857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" s="2" t="s">
         <v>758</v>
       </c>
@@ -7977,7 +7977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A173" s="2" t="s">
         <v>773</v>
       </c>
@@ -8125,8 +8125,8 @@
       <c r="A191" s="2" t="s">
         <v>791</v>
       </c>
-      <c r="B191" t="s">
-        <v>902</v>
+      <c r="B191">
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
@@ -8566,7 +8566,7 @@
         <v>846</v>
       </c>
       <c r="B246">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
@@ -8622,7 +8622,7 @@
         <v>853</v>
       </c>
       <c r="B253">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="87" x14ac:dyDescent="0.35">
@@ -8702,7 +8702,7 @@
         <v>863</v>
       </c>
       <c r="B263">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.35">
@@ -8710,7 +8710,7 @@
         <v>864</v>
       </c>
       <c r="B264">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
@@ -8726,7 +8726,7 @@
         <v>866</v>
       </c>
       <c r="B266">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
@@ -8926,7 +8926,7 @@
         <v>891</v>
       </c>
       <c r="B291">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="58" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Função de limpeza melhorada e atualizada, processo de limpeza e de criação de listas para os tweets irrelevantes realizado, excel com classificação melhorada
</commit_message>
<xml_diff>
--- a/Airpods.xlsx
+++ b/Airpods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liviabn\Documents\Cdados- Projetos\PROJETO1_Cdados\P1Cdados2021_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5FEC3E9-F363-445C-B2AD-DCBA4C6F2050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{938E5928-1DA8-488E-8586-543DB4F5C94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3575,8 +3575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B601"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A556" workbookViewId="0">
-      <selection activeCell="B564" sqref="B564"/>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="B252" sqref="B252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3958,7 +3958,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -3990,7 +3990,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -4014,7 +4014,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="116.1">
@@ -4038,7 +4038,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -4070,7 +4070,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="116.1">
@@ -4102,7 +4102,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="29.1">
@@ -4214,7 +4214,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -4222,7 +4222,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="101.45">
@@ -4254,7 +4254,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -4278,7 +4278,7 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -4302,7 +4302,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -4334,7 +4334,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -4382,7 +4382,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="29.1">
@@ -4406,7 +4406,7 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -4438,7 +4438,7 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -4454,7 +4454,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -4462,7 +4462,7 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -4470,7 +4470,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -4478,7 +4478,7 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -4510,7 +4510,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -4558,7 +4558,7 @@
         <v>122</v>
       </c>
       <c r="B122">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="57.95">
@@ -4622,7 +4622,7 @@
         <v>130</v>
       </c>
       <c r="B130">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="43.5">
@@ -4646,7 +4646,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -4670,7 +4670,7 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="29.1">
@@ -4694,7 +4694,7 @@
         <v>139</v>
       </c>
       <c r="B139">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="144.94999999999999">
@@ -4718,7 +4718,7 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -4774,7 +4774,7 @@
         <v>149</v>
       </c>
       <c r="B149">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="43.5">
@@ -4814,7 +4814,7 @@
         <v>154</v>
       </c>
       <c r="B154">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -4846,7 +4846,7 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -4878,7 +4878,7 @@
         <v>162</v>
       </c>
       <c r="B162">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -4918,7 +4918,7 @@
         <v>167</v>
       </c>
       <c r="B167">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -4950,7 +4950,7 @@
         <v>171</v>
       </c>
       <c r="B171">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -4990,7 +4990,7 @@
         <v>176</v>
       </c>
       <c r="B176">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="29.1">
@@ -5014,7 +5014,7 @@
         <v>179</v>
       </c>
       <c r="B179">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="29.1">
@@ -5022,7 +5022,7 @@
         <v>180</v>
       </c>
       <c r="B180">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -5134,7 +5134,7 @@
         <v>194</v>
       </c>
       <c r="B194">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -5198,7 +5198,7 @@
         <v>202</v>
       </c>
       <c r="B202">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -5590,7 +5590,7 @@
         <v>251</v>
       </c>
       <c r="B251">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252" spans="1:2">

</xml_diff>

<commit_message>
Excel revisado de novo
</commit_message>
<xml_diff>
--- a/Airpods.xlsx
+++ b/Airpods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liviabn\Documents\Cdados- Projetos\PROJETO1_Cdados\P1Cdados2021_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5457F924-D02E-4201-A443-94E839F50721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B5DF0A-9DF2-4A4F-AA2D-3F3771148D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3580,11 +3580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:B601"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="B241" sqref="B241"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3609,7 +3608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3617,7 +3616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -3633,7 +3632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -3641,7 +3640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -3657,7 +3656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -3697,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -3737,7 +3736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -3769,7 +3768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -3777,7 +3776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -3793,7 +3792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -3841,7 +3840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -3849,7 +3848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -3961,7 +3960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -3977,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
@@ -3993,7 +3992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
@@ -4001,7 +4000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -4017,7 +4016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
@@ -4033,7 +4032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
@@ -4041,7 +4040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
@@ -4065,7 +4064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
@@ -4073,7 +4072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
@@ -4089,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
@@ -4105,7 +4104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
@@ -4121,7 +4120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
@@ -4137,7 +4136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>68</v>
       </c>
@@ -4153,7 +4152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
@@ -4193,7 +4192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
@@ -4217,7 +4216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -4225,7 +4224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
@@ -4257,7 +4256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>83</v>
       </c>
@@ -4281,7 +4280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>86</v>
       </c>
@@ -4305,7 +4304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>89</v>
       </c>
@@ -4337,7 +4336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>93</v>
       </c>
@@ -4361,7 +4360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
@@ -4385,7 +4384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>99</v>
       </c>
@@ -4409,7 +4408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>102</v>
       </c>
@@ -4417,7 +4416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>103</v>
       </c>
@@ -4425,7 +4424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>104</v>
       </c>
@@ -4433,7 +4432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>105</v>
       </c>
@@ -4441,7 +4440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>106</v>
       </c>
@@ -4449,7 +4448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>107</v>
       </c>
@@ -4457,7 +4456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>108</v>
       </c>
@@ -4465,7 +4464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
         <v>109</v>
       </c>
@@ -4473,7 +4472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>110</v>
       </c>
@@ -4481,7 +4480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>111</v>
       </c>
@@ -4505,7 +4504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>114</v>
       </c>
@@ -4513,7 +4512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
         <v>115</v>
       </c>
@@ -4521,7 +4520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>116</v>
       </c>
@@ -4529,7 +4528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>117</v>
       </c>
@@ -4561,7 +4560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>121</v>
       </c>
@@ -4593,7 +4592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>125</v>
       </c>
@@ -4601,7 +4600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>126</v>
       </c>
@@ -4625,7 +4624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
         <v>129</v>
       </c>
@@ -4649,7 +4648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>132</v>
       </c>
@@ -4673,7 +4672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>135</v>
       </c>
@@ -4697,7 +4696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="116" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>138</v>
       </c>
@@ -4721,7 +4720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="s">
         <v>141</v>
       </c>
@@ -4737,7 +4736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
         <v>143</v>
       </c>
@@ -4769,7 +4768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" s="2" t="s">
         <v>147</v>
       </c>
@@ -4777,7 +4776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A149" s="2" t="s">
         <v>148</v>
       </c>
@@ -4793,7 +4792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" s="2" t="s">
         <v>150</v>
       </c>
@@ -4817,7 +4816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" s="2" t="s">
         <v>153</v>
       </c>
@@ -4849,7 +4848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A158" s="2" t="s">
         <v>157</v>
       </c>
@@ -4881,7 +4880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A162" s="2" t="s">
         <v>161</v>
       </c>
@@ -4921,7 +4920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="2" t="s">
         <v>166</v>
       </c>
@@ -4937,7 +4936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A169" s="2" t="s">
         <v>168</v>
       </c>
@@ -4953,7 +4952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="116" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A171" s="2" t="s">
         <v>170</v>
       </c>
@@ -4993,7 +4992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A176" s="2" t="s">
         <v>175</v>
       </c>
@@ -5017,7 +5016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" s="2" t="s">
         <v>178</v>
       </c>
@@ -5025,7 +5024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A180" s="2" t="s">
         <v>179</v>
       </c>
@@ -5081,7 +5080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" s="2" t="s">
         <v>186</v>
       </c>
@@ -5113,7 +5112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" s="2" t="s">
         <v>190</v>
       </c>
@@ -5137,7 +5136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" s="2" t="s">
         <v>193</v>
       </c>
@@ -5201,7 +5200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A202" s="2" t="s">
         <v>201</v>
       </c>
@@ -5233,7 +5232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" s="2" t="s">
         <v>205</v>
       </c>
@@ -5265,7 +5264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" s="2" t="s">
         <v>209</v>
       </c>
@@ -5297,7 +5296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A214" s="2" t="s">
         <v>213</v>
       </c>
@@ -5353,7 +5352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" s="2" t="s">
         <v>220</v>
       </c>
@@ -5425,7 +5424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" s="2" t="s">
         <v>229</v>
       </c>
@@ -5433,7 +5432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" s="2" t="s">
         <v>230</v>
       </c>
@@ -5457,7 +5456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A234" s="2" t="s">
         <v>233</v>
       </c>
@@ -5465,7 +5464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A235" s="2" t="s">
         <v>234</v>
       </c>
@@ -5473,7 +5472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A236" s="2" t="s">
         <v>235</v>
       </c>
@@ -5497,7 +5496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" s="2" t="s">
         <v>238</v>
       </c>
@@ -5529,7 +5528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" s="2" t="s">
         <v>242</v>
       </c>
@@ -5545,7 +5544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" s="2" t="s">
         <v>244</v>
       </c>
@@ -5553,7 +5552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" s="2" t="s">
         <v>245</v>
       </c>
@@ -5561,7 +5560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" s="2" t="s">
         <v>246</v>
       </c>
@@ -5593,7 +5592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" s="2" t="s">
         <v>250</v>
       </c>
@@ -5601,7 +5600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" s="2" t="s">
         <v>251</v>
       </c>
@@ -5617,7 +5616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" s="2" t="s">
         <v>253</v>
       </c>
@@ -5625,7 +5624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A255" s="2" t="s">
         <v>254</v>
       </c>
@@ -5641,7 +5640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" s="2" t="s">
         <v>256</v>
       </c>
@@ -5665,7 +5664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" s="2" t="s">
         <v>259</v>
       </c>
@@ -5705,7 +5704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" s="2" t="s">
         <v>264</v>
       </c>
@@ -5758,10 +5757,10 @@
         <v>270</v>
       </c>
       <c r="B271" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" s="2" t="s">
         <v>271</v>
       </c>
@@ -5774,7 +5773,7 @@
         <v>272</v>
       </c>
       <c r="B273" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.35">
@@ -5785,7 +5784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A275" s="2" t="s">
         <v>274</v>
       </c>
@@ -5809,7 +5808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A278" s="2" t="s">
         <v>277</v>
       </c>
@@ -5889,7 +5888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288" s="2" t="s">
         <v>287</v>
       </c>
@@ -5913,7 +5912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A291" s="2" t="s">
         <v>290</v>
       </c>
@@ -6025,7 +6024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A305" s="2" t="s">
         <v>304</v>
       </c>
@@ -6129,7 +6128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A318" s="2" t="s">
         <v>317</v>
       </c>
@@ -6153,7 +6152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A321" s="2" t="s">
         <v>320</v>
       </c>
@@ -6174,10 +6173,10 @@
         <v>322</v>
       </c>
       <c r="B323" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A324" s="2" t="s">
         <v>323</v>
       </c>
@@ -6209,7 +6208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A328" s="2" t="s">
         <v>327</v>
       </c>
@@ -6273,7 +6272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A336" s="2" t="s">
         <v>335</v>
       </c>
@@ -6361,7 +6360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A347" s="2" t="s">
         <v>346</v>
       </c>
@@ -6369,7 +6368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A348" s="2" t="s">
         <v>347</v>
       </c>
@@ -6377,7 +6376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:2" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A349" s="2" t="s">
         <v>348</v>
       </c>
@@ -6385,7 +6384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A350" s="2" t="s">
         <v>349</v>
       </c>
@@ -6398,7 +6397,7 @@
         <v>350</v>
       </c>
       <c r="B351" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="87" x14ac:dyDescent="0.35">
@@ -6441,7 +6440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A357" s="2" t="s">
         <v>356</v>
       </c>
@@ -6449,7 +6448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358" s="2" t="s">
         <v>357</v>
       </c>
@@ -6457,7 +6456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:2" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A359" s="2" t="s">
         <v>358</v>
       </c>
@@ -6481,7 +6480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" s="2" t="s">
         <v>361</v>
       </c>
@@ -6505,7 +6504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" s="2" t="s">
         <v>364</v>
       </c>
@@ -6513,7 +6512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" s="2" t="s">
         <v>365</v>
       </c>
@@ -6521,7 +6520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" s="2" t="s">
         <v>366</v>
       </c>
@@ -6569,7 +6568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A373" s="2" t="s">
         <v>372</v>
       </c>
@@ -6617,7 +6616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A379" s="2" t="s">
         <v>378</v>
       </c>
@@ -6625,7 +6624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" s="2" t="s">
         <v>379</v>
       </c>
@@ -6633,7 +6632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A381" s="2" t="s">
         <v>380</v>
       </c>
@@ -6641,7 +6640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" s="2" t="s">
         <v>381</v>
       </c>
@@ -6649,7 +6648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" s="2" t="s">
         <v>382</v>
       </c>
@@ -6657,7 +6656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" s="2" t="s">
         <v>383</v>
       </c>
@@ -6673,7 +6672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" s="2" t="s">
         <v>385</v>
       </c>
@@ -6697,7 +6696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" s="2" t="s">
         <v>388</v>
       </c>
@@ -6721,7 +6720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" s="2" t="s">
         <v>391</v>
       </c>
@@ -6745,7 +6744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:2" ht="116" hidden="1" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A395" s="2" t="s">
         <v>394</v>
       </c>
@@ -6769,7 +6768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A398" s="2" t="s">
         <v>397</v>
       </c>
@@ -6777,7 +6776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="399" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A399" s="2" t="s">
         <v>398</v>
       </c>
@@ -6809,7 +6808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A403" s="2" t="s">
         <v>402</v>
       </c>
@@ -6825,7 +6824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A405" s="2" t="s">
         <v>404</v>
       </c>
@@ -6862,7 +6861,7 @@
         <v>408</v>
       </c>
       <c r="B409" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="58" x14ac:dyDescent="0.35">
@@ -6889,7 +6888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:2" ht="159.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A413" s="2" t="s">
         <v>412</v>
       </c>
@@ -6902,7 +6901,7 @@
         <v>413</v>
       </c>
       <c r="B414" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="116" x14ac:dyDescent="0.35">
@@ -6913,7 +6912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:2" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A416" s="2" t="s">
         <v>415</v>
       </c>
@@ -6929,7 +6928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A418" s="2" t="s">
         <v>417</v>
       </c>
@@ -6953,7 +6952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:2" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A421" s="2" t="s">
         <v>420</v>
       </c>
@@ -6961,7 +6960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="422" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A422" s="2" t="s">
         <v>421</v>
       </c>
@@ -6977,7 +6976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A424" s="2" t="s">
         <v>423</v>
       </c>
@@ -7017,7 +7016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:2" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A429" s="2" t="s">
         <v>428</v>
       </c>
@@ -7038,10 +7037,10 @@
         <v>430</v>
       </c>
       <c r="B431" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="432" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A432" s="2" t="s">
         <v>431</v>
       </c>
@@ -7065,7 +7064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="435" spans="1:2" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A435" s="2" t="s">
         <v>434</v>
       </c>
@@ -7081,7 +7080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:2" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A437" s="2" t="s">
         <v>436</v>
       </c>
@@ -7121,7 +7120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A442" s="2" t="s">
         <v>441</v>
       </c>
@@ -7137,7 +7136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="444" spans="1:2" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="444" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A444" s="2" t="s">
         <v>443</v>
       </c>
@@ -7145,7 +7144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="445" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A445" s="2" t="s">
         <v>444</v>
       </c>
@@ -7161,7 +7160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A447" s="2" t="s">
         <v>446</v>
       </c>
@@ -7177,7 +7176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A449" s="2" t="s">
         <v>448</v>
       </c>
@@ -7217,7 +7216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="454" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A454" s="2" t="s">
         <v>453</v>
       </c>
@@ -7233,7 +7232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="456" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A456" s="2" t="s">
         <v>455</v>
       </c>
@@ -7257,7 +7256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="459" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="459" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A459" s="2" t="s">
         <v>458</v>
       </c>
@@ -7281,7 +7280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="462" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="462" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A462" s="2" t="s">
         <v>461</v>
       </c>
@@ -7289,7 +7288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="463" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="463" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A463" s="2" t="s">
         <v>462</v>
       </c>
@@ -7305,7 +7304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="465" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="465" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A465" s="2" t="s">
         <v>464</v>
       </c>
@@ -7342,10 +7341,10 @@
         <v>468</v>
       </c>
       <c r="B469" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="470" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A470" s="2" t="s">
         <v>469</v>
       </c>
@@ -7353,7 +7352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="471" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="471" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A471" s="2" t="s">
         <v>470</v>
       </c>
@@ -7377,7 +7376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="474" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="474" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A474" s="2" t="s">
         <v>473</v>
       </c>
@@ -7393,7 +7392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="476" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="476" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A476" s="2" t="s">
         <v>475</v>
       </c>
@@ -7433,7 +7432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="481" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A481" s="2" t="s">
         <v>480</v>
       </c>
@@ -7449,7 +7448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="483" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="483" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A483" s="2" t="s">
         <v>482</v>
       </c>
@@ -7457,7 +7456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="484" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="484" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A484" s="2" t="s">
         <v>483</v>
       </c>
@@ -7473,7 +7472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="486" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="486" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A486" s="2" t="s">
         <v>485</v>
       </c>
@@ -7481,7 +7480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="487" spans="1:2" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="487" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A487" s="2" t="s">
         <v>486</v>
       </c>
@@ -7489,7 +7488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="488" spans="1:2" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="488" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A488" s="2" t="s">
         <v>487</v>
       </c>
@@ -7513,7 +7512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="491" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="491" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A491" s="2" t="s">
         <v>490</v>
       </c>
@@ -7521,7 +7520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="492" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="492" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A492" s="2" t="s">
         <v>491</v>
       </c>
@@ -7529,7 +7528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="493" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="493" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A493" s="2" t="s">
         <v>492</v>
       </c>
@@ -7537,7 +7536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="494" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="494" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A494" s="2" t="s">
         <v>493</v>
       </c>
@@ -7601,7 +7600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="502" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="502" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A502" s="2" t="s">
         <v>501</v>
       </c>
@@ -7609,7 +7608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="503" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="503" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A503" s="2" t="s">
         <v>502</v>
       </c>
@@ -7673,7 +7672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="511" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="511" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A511" s="2" t="s">
         <v>510</v>
       </c>
@@ -7697,7 +7696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="514" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="514" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A514" s="2" t="s">
         <v>513</v>
       </c>
@@ -7713,7 +7712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="516" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="516" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A516" s="2" t="s">
         <v>515</v>
       </c>
@@ -7721,7 +7720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="517" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="517" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A517" s="2" t="s">
         <v>516</v>
       </c>
@@ -7753,7 +7752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="521" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="521" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A521" s="2" t="s">
         <v>520</v>
       </c>
@@ -7769,7 +7768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="523" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="523" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A523" s="2" t="s">
         <v>522</v>
       </c>
@@ -7809,7 +7808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="528" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="528" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A528" s="2" t="s">
         <v>527</v>
       </c>
@@ -7817,7 +7816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="529" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="529" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A529" s="2" t="s">
         <v>528</v>
       </c>
@@ -7825,7 +7824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="530" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="530" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A530" s="2" t="s">
         <v>529</v>
       </c>
@@ -7849,7 +7848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="533" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="533" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A533" s="2" t="s">
         <v>532</v>
       </c>
@@ -7889,7 +7888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="538" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="538" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A538" s="2" t="s">
         <v>537</v>
       </c>
@@ -7897,7 +7896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="539" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="539" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A539" s="2" t="s">
         <v>538</v>
       </c>
@@ -7921,7 +7920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="542" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="542" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A542" s="2" t="s">
         <v>541</v>
       </c>
@@ -7961,7 +7960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="547" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="547" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A547" s="2" t="s">
         <v>546</v>
       </c>
@@ -7977,7 +7976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="549" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="549" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A549" s="2" t="s">
         <v>548</v>
       </c>
@@ -8033,7 +8032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="556" spans="1:2" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="556" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A556" s="2" t="s">
         <v>555</v>
       </c>
@@ -8049,7 +8048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="558" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="558" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A558" s="2" t="s">
         <v>557</v>
       </c>
@@ -8081,7 +8080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="562" spans="1:2" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="562" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A562" s="2" t="s">
         <v>561</v>
       </c>
@@ -8113,7 +8112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="566" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="566" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A566" s="2" t="s">
         <v>565</v>
       </c>
@@ -8145,7 +8144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="570" spans="1:2" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="570" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A570" s="2" t="s">
         <v>569</v>
       </c>
@@ -8201,7 +8200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="577" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="577" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A577" s="2" t="s">
         <v>576</v>
       </c>
@@ -8233,7 +8232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="581" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="581" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A581" s="2" t="s">
         <v>580</v>
       </c>
@@ -8257,7 +8256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="584" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="584" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A584" s="2" t="s">
         <v>583</v>
       </c>
@@ -8265,7 +8264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="585" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="585" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A585" s="2" t="s">
         <v>584</v>
       </c>
@@ -8329,7 +8328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="593" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="593" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A593" s="2" t="s">
         <v>592</v>
       </c>
@@ -8345,7 +8344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="595" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="595" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A595" s="2" t="s">
         <v>594</v>
       </c>
@@ -8353,7 +8352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="596" spans="1:2" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="596" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A596" s="2" t="s">
         <v>595</v>
       </c>
@@ -8369,7 +8368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="598" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="598" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A598" s="2" t="s">
         <v>597</v>
       </c>
@@ -8402,13 +8401,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B601" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="0"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:B601" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>